<commit_message>
Corrected concentration vs altitude measurements for instantaneous mass flow rate which is logged by the sensor
</commit_message>
<xml_diff>
--- a/data/HASP_2018/MURI_HASP_2018_Data_no_calibration.xlsx
+++ b/data/HASP_2018/MURI_HASP_2018_Data_no_calibration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\MURI_HAB\Data_Analysis\data\HASP_2018\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F3634CEA-4F34-4122-BAD9-9ADCEEB83F99}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{91A6BDE7-271B-4B0F-BE05-6C2A4F9CBFC3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16560" windowHeight="10988" xr2:uid="{66F0F296-1776-4ED1-B60C-48C1F1D78A3C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="10988" xr2:uid="{900E5CC6-CE8E-40EC-BE86-3A838A69E185}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,55 +27,58 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
-    <t>80000-82500</t>
-  </si>
-  <si>
-    <t>82500-85000</t>
-  </si>
-  <si>
-    <t>85000-87500</t>
-  </si>
-  <si>
-    <t>87500-90000</t>
-  </si>
-  <si>
-    <t>90000-92500</t>
-  </si>
-  <si>
-    <t>92500-95000</t>
-  </si>
-  <si>
-    <t>95000-97500</t>
-  </si>
-  <si>
-    <t>97500-100000</t>
-  </si>
-  <si>
-    <t>100000-102500</t>
-  </si>
-  <si>
-    <t>102500-105000</t>
-  </si>
-  <si>
-    <t>105000-107500</t>
-  </si>
-  <si>
-    <t>107500-110000</t>
-  </si>
-  <si>
-    <t>110000-112500</t>
-  </si>
-  <si>
-    <t>112500-115000</t>
-  </si>
-  <si>
-    <t>115000-117500</t>
-  </si>
-  <si>
-    <t>117500-120000</t>
-  </si>
-  <si>
-    <t>120000-122500</t>
+    <t>'80000-82500'</t>
+  </si>
+  <si>
+    <t>'82500-85000'</t>
+  </si>
+  <si>
+    <t>'85000-87500'</t>
+  </si>
+  <si>
+    <t>'87500-90000'</t>
+  </si>
+  <si>
+    <t>'90000-92500'</t>
+  </si>
+  <si>
+    <t>'92500-95000'</t>
+  </si>
+  <si>
+    <t>'95000-97500'</t>
+  </si>
+  <si>
+    <t>'97500-100000'</t>
+  </si>
+  <si>
+    <t>'100000-102500'</t>
+  </si>
+  <si>
+    <t>'102500-105000'</t>
+  </si>
+  <si>
+    <t>'105000-107500'</t>
+  </si>
+  <si>
+    <t>'107500-110000'</t>
+  </si>
+  <si>
+    <t>'110000-112500'</t>
+  </si>
+  <si>
+    <t>'112500-115000'</t>
+  </si>
+  <si>
+    <t>'115000-117500'</t>
+  </si>
+  <si>
+    <t>'117500-120000'</t>
+  </si>
+  <si>
+    <t>'120000-122500'</t>
+  </si>
+  <si>
+    <t>Altitude Range (ft)</t>
   </si>
   <si>
     <t>0.35-0.54 (um)</t>
@@ -87,12 +90,6 @@
     <t>0.78-1.0 (um)</t>
   </si>
   <si>
-    <t>Concentrations in particles/cm^3 normalized for bin width (dN/dlog(D))</t>
-  </si>
-  <si>
-    <t>Altitude Range (ft)</t>
-  </si>
-  <si>
     <t>1.0-1.3 (um)</t>
   </si>
   <si>
@@ -130,6 +127,9 @@
   </si>
   <si>
     <t>16.0-Max (um)</t>
+  </si>
+  <si>
+    <t>*concentration in particles/cm^3</t>
   </si>
 </sst>
 </file>
@@ -165,9 +165,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -484,84 +483,82 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A6BCC5C-91C1-430D-8AD1-70A628CDCB2A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41FD1421-A69F-435D-8FB6-C46987DEE2FD}">
   <dimension ref="A1:Q20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="15.796875" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" customWidth="1"/>
-    <col min="4" max="4" width="12.73046875" customWidth="1"/>
-    <col min="5" max="5" width="13.86328125" customWidth="1"/>
-    <col min="6" max="6" width="13.19921875" customWidth="1"/>
-    <col min="7" max="7" width="11.796875" customWidth="1"/>
-    <col min="8" max="8" width="12" customWidth="1"/>
-    <col min="9" max="9" width="11.6640625" customWidth="1"/>
-    <col min="10" max="10" width="11.265625" customWidth="1"/>
-    <col min="11" max="11" width="12.9296875" customWidth="1"/>
-    <col min="12" max="12" width="13.59765625" customWidth="1"/>
-    <col min="13" max="13" width="13.06640625" customWidth="1"/>
+    <col min="1" max="1" width="15.86328125" customWidth="1"/>
+    <col min="2" max="3" width="12.19921875" customWidth="1"/>
+    <col min="4" max="4" width="12.1328125" customWidth="1"/>
+    <col min="5" max="5" width="12.265625" customWidth="1"/>
+    <col min="6" max="6" width="11.06640625" customWidth="1"/>
+    <col min="7" max="8" width="11.265625" customWidth="1"/>
+    <col min="9" max="9" width="11.73046875" customWidth="1"/>
+    <col min="10" max="11" width="10.86328125" customWidth="1"/>
+    <col min="12" max="12" width="11.19921875" customWidth="1"/>
+    <col min="13" max="13" width="11.796875" customWidth="1"/>
     <col min="14" max="14" width="13.1328125" customWidth="1"/>
-    <col min="15" max="17" width="13.19921875" customWidth="1"/>
-    <col min="18" max="18" width="11.46484375" customWidth="1"/>
+    <col min="15" max="15" width="12.33203125" customWidth="1"/>
+    <col min="16" max="16" width="12.9296875" customWidth="1"/>
+    <col min="17" max="17" width="11.1328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.45">
@@ -569,13 +566,13 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.11651232702764</v>
+        <v>0.21203448647536699</v>
       </c>
       <c r="C2">
-        <v>5.5364036161166903E-3</v>
+        <v>1.40855585854841E-2</v>
       </c>
       <c r="D2">
-        <v>2.7691141619700402E-4</v>
+        <v>5.9171347033270703E-4</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -590,7 +587,7 @@
         <v>0</v>
       </c>
       <c r="I2">
-        <v>2.4386170636181599E-4</v>
+        <v>6.1088759731221397E-4</v>
       </c>
       <c r="J2">
         <v>0</v>
@@ -618,17 +615,17 @@
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.140007496035154</v>
+        <v>0.37394762185769698</v>
       </c>
       <c r="C3">
-        <v>5.8787213998799104E-3</v>
+        <v>1.5053507654185901E-2</v>
       </c>
       <c r="D3">
-        <v>2.7691141619700402E-4</v>
+        <v>5.9716362028008798E-4</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -643,7 +640,7 @@
         <v>0</v>
       </c>
       <c r="I3">
-        <v>2.4386170636181599E-4</v>
+        <v>6.1651435616303903E-4</v>
       </c>
       <c r="J3">
         <v>0</v>
@@ -675,13 +672,13 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>7.6017101374066601E-2</v>
+        <v>0.26010644613371398</v>
       </c>
       <c r="C4">
-        <v>5.5364036161166903E-3</v>
+        <v>1.4215297741735401E-2</v>
       </c>
       <c r="D4">
-        <v>5.6922874731534E-4</v>
+        <v>1.3013825237058799E-3</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -696,7 +693,7 @@
         <v>0</v>
       </c>
       <c r="I4">
-        <v>2.4386170636181599E-4</v>
+        <v>6.1651435616303903E-4</v>
       </c>
       <c r="J4">
         <v>0</v>
@@ -728,13 +725,13 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.10166853120984801</v>
+        <v>0.28322780644525403</v>
       </c>
       <c r="C5">
-        <v>5.5364036161166903E-3</v>
+        <v>1.4215297741735401E-2</v>
       </c>
       <c r="D5">
-        <v>2.7691141619700402E-4</v>
+        <v>5.9716362028008798E-4</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -749,7 +746,7 @@
         <v>0</v>
       </c>
       <c r="I5">
-        <v>2.4386170636181599E-4</v>
+        <v>6.1651435616303903E-4</v>
       </c>
       <c r="J5">
         <v>0</v>
@@ -781,13 +778,13 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>0.10166853120984801</v>
+        <v>0.28322780644525403</v>
       </c>
       <c r="C6">
-        <v>5.5364036161166903E-3</v>
+        <v>1.4215297741735401E-2</v>
       </c>
       <c r="D6">
-        <v>2.7691141619700402E-4</v>
+        <v>5.9716362028008798E-4</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -802,7 +799,7 @@
         <v>0</v>
       </c>
       <c r="I6">
-        <v>2.4386170636181599E-4</v>
+        <v>6.1651435616303903E-4</v>
       </c>
       <c r="J6">
         <v>0</v>
@@ -834,13 +831,13 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>0.10166853120984801</v>
+        <v>0.28322780644525403</v>
       </c>
       <c r="C7">
-        <v>5.5364036161166903E-3</v>
+        <v>1.4215297741735401E-2</v>
       </c>
       <c r="D7">
-        <v>2.7691141619700402E-4</v>
+        <v>5.9716362028008798E-4</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -855,7 +852,7 @@
         <v>0</v>
       </c>
       <c r="I7">
-        <v>2.4386170636181599E-4</v>
+        <v>6.1651435616303903E-4</v>
       </c>
       <c r="J7">
         <v>0</v>
@@ -887,13 +884,13 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>0.112352105637962</v>
+        <v>0.28395592933575498</v>
       </c>
       <c r="C8">
-        <v>5.5364036161166903E-3</v>
+        <v>1.4215297741735401E-2</v>
       </c>
       <c r="D8">
-        <v>2.7691141619700402E-4</v>
+        <v>5.9716362028008798E-4</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -908,7 +905,7 @@
         <v>0</v>
       </c>
       <c r="I8">
-        <v>2.4386170636181599E-4</v>
+        <v>6.1651435616303903E-4</v>
       </c>
       <c r="J8">
         <v>0</v>
@@ -940,13 +937,13 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>4.1682289478922399E-2</v>
+        <v>0.23212374735216501</v>
       </c>
       <c r="C9">
-        <v>5.5364036161166903E-3</v>
+        <v>1.4215297741735401E-2</v>
       </c>
       <c r="D9">
-        <v>2.7691141619700402E-4</v>
+        <v>5.9716362028008798E-4</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -961,7 +958,7 @@
         <v>0</v>
       </c>
       <c r="I9">
-        <v>2.4386170636181599E-4</v>
+        <v>6.1651435616303903E-4</v>
       </c>
       <c r="J9">
         <v>0</v>
@@ -993,13 +990,13 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>0.14191080372995499</v>
+        <v>0.32735806932985301</v>
       </c>
       <c r="C10">
-        <v>5.5364036161166903E-3</v>
+        <v>1.4215297741735401E-2</v>
       </c>
       <c r="D10">
-        <v>2.7691141619700402E-4</v>
+        <v>5.9716362028008798E-4</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -1014,7 +1011,7 @@
         <v>0</v>
       </c>
       <c r="I10">
-        <v>2.4386170636181599E-4</v>
+        <v>6.1651435616303903E-4</v>
       </c>
       <c r="J10">
         <v>0</v>
@@ -1046,13 +1043,13 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>8.3684318892864304E-2</v>
+        <v>0.26417667782090798</v>
       </c>
       <c r="C11">
-        <v>5.5364036161166903E-3</v>
+        <v>1.4215297741735401E-2</v>
       </c>
       <c r="D11">
-        <v>2.7691141619700402E-4</v>
+        <v>5.9716362028008798E-4</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -1067,7 +1064,7 @@
         <v>0</v>
       </c>
       <c r="I11">
-        <v>2.4386170636181599E-4</v>
+        <v>6.1651435616303903E-4</v>
       </c>
       <c r="J11">
         <v>0</v>
@@ -1099,13 +1096,13 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>0.11407825515664601</v>
+        <v>0.35155278910322502</v>
       </c>
       <c r="C12">
-        <v>5.5364036161166903E-3</v>
+        <v>1.4215297741735401E-2</v>
       </c>
       <c r="D12">
-        <v>2.7691141619700402E-4</v>
+        <v>5.9716362028008798E-4</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -1120,7 +1117,7 @@
         <v>0</v>
       </c>
       <c r="I12">
-        <v>2.4386170636181599E-4</v>
+        <v>6.1651435616303903E-4</v>
       </c>
       <c r="J12">
         <v>0</v>
@@ -1152,13 +1149,13 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>0.110178587380191</v>
+        <v>0.325218214921763</v>
       </c>
       <c r="C13">
-        <v>5.5364036161166903E-3</v>
+        <v>1.4215297741735401E-2</v>
       </c>
       <c r="D13">
-        <v>2.7691141619700402E-4</v>
+        <v>5.9716362028008798E-4</v>
       </c>
       <c r="E13">
         <v>0</v>
@@ -1173,7 +1170,7 @@
         <v>0</v>
       </c>
       <c r="I13">
-        <v>2.4386170636181599E-4</v>
+        <v>6.1651435616303903E-4</v>
       </c>
       <c r="J13">
         <v>0</v>
@@ -1205,13 +1202,13 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>9.55292148501342E-2</v>
+        <v>0.21102670953128</v>
       </c>
       <c r="C14">
-        <v>5.5364036161166903E-3</v>
+        <v>1.4215297741735401E-2</v>
       </c>
       <c r="D14">
-        <v>2.7691141619700402E-4</v>
+        <v>5.9716362028008798E-4</v>
       </c>
       <c r="E14">
         <v>0</v>
@@ -1226,7 +1223,7 @@
         <v>0</v>
       </c>
       <c r="I14">
-        <v>2.4386170636181599E-4</v>
+        <v>6.1651435616303903E-4</v>
       </c>
       <c r="J14">
         <v>0</v>
@@ -1258,13 +1255,13 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>6.3404950467238694E-2</v>
+        <v>0.14579317291712701</v>
       </c>
       <c r="C15">
-        <v>5.3514722546476696E-3</v>
+        <v>1.3301308172691E-2</v>
       </c>
       <c r="D15">
-        <v>2.7691141619700402E-4</v>
+        <v>5.9716362028008798E-4</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -1279,7 +1276,7 @@
         <v>0</v>
       </c>
       <c r="I15">
-        <v>2.4386170636181599E-4</v>
+        <v>6.1651435616303903E-4</v>
       </c>
       <c r="J15">
         <v>0</v>
@@ -1311,13 +1308,13 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>5.4678023966238901E-2</v>
+        <v>0.14401253625171601</v>
       </c>
       <c r="C16">
-        <v>5.3514722546476696E-3</v>
+        <v>1.3301308172691E-2</v>
       </c>
       <c r="D16">
-        <v>2.7691141619700402E-4</v>
+        <v>5.9716362028008798E-4</v>
       </c>
       <c r="E16">
         <v>0</v>
@@ -1332,7 +1329,7 @@
         <v>0</v>
       </c>
       <c r="I16">
-        <v>2.4386170636181599E-4</v>
+        <v>6.1651435616303903E-4</v>
       </c>
       <c r="J16">
         <v>0</v>
@@ -1364,7 +1361,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>1.43929701515026E-2</v>
+        <v>2.8896228977663699E-2</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -1385,7 +1382,7 @@
         <v>0</v>
       </c>
       <c r="I17">
-        <v>2.4386170636181599E-4</v>
+        <v>5.2882577892819703E-4</v>
       </c>
       <c r="J17">
         <v>0</v>
@@ -1417,10 +1414,10 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>5.9679027072216204E-3</v>
+        <v>1.4875778803152301E-2</v>
       </c>
       <c r="C18">
-        <v>1.8710130671675999E-4</v>
+        <v>4.0348677281917101E-4</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -1435,7 +1432,7 @@
         <v>0</v>
       </c>
       <c r="H18">
-        <v>1.96690690697482E-4</v>
+        <v>4.9725984595016702E-4</v>
       </c>
       <c r="I18">
         <v>0</v>
@@ -1466,8 +1463,8 @@
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="B20" t="s">
-        <v>20</v>
+      <c r="A20" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>